<commit_message>
Parse command line arguments editted
</commit_message>
<xml_diff>
--- a/global_results.xlsx
+++ b/global_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,7 +450,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>90.17</v>
+        <v>45.05</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>95.97</v>
+        <v>89.68000000000001</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>96.89</v>
+        <v>88.61</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>97.23</v>
+        <v>93.18000000000001</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,47 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>97.42</v>
+        <v>94.47</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>95.61</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>95.91</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>96.11</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>96.18000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add cifar, but not working right now
</commit_message>
<xml_diff>
--- a/global_results.xlsx
+++ b/global_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,79 +450,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>82.11</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>95.3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>96.39</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>96.34999999999999</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>97.26000000000001</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>97.31999999999999</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>97.56999999999999</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>97.75</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>97.92</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="n">
-        <v>97.98999999999999</v>
+        <v>10.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>